<commit_message>
Fixed "Plaintiff" spelling error
</commit_message>
<xml_diff>
--- a/Documents/inputCsvExample.xlsx
+++ b/Documents/inputCsvExample.xlsx
@@ -223,9 +223,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Palintiff, Defendant</t>
-  </si>
-  <si>
     <t>Participant Hard Limit</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>Preferred Partners</t>
+  </si>
+  <si>
+    <t>Plaintiff, Defendant</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -785,13 +785,13 @@
         <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -944,10 +944,10 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,10 +958,10 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -969,13 +969,13 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -986,10 +986,10 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,10 +1000,10 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>